<commit_message>
Checking in new process to add to postgres
</commit_message>
<xml_diff>
--- a/Leetcode.xlsx
+++ b/Leetcode.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16c6da65896e9738/Desktop/DD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A5218E7-3BD7-4F7F-B655-219AB2D9D218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{7A5218E7-3BD7-4F7F-B655-219AB2D9D218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9EA7E7F-594B-465C-8F78-E815293E5421}"/>
   <bookViews>
-    <workbookView xWindow="-23040" yWindow="1092" windowWidth="28800" windowHeight="11388" activeTab="5" xr2:uid="{550F2F40-7B1A-46CC-9BB7-B3D78208C6B1}"/>
+    <workbookView minimized="1" xWindow="-32376" yWindow="1560" windowWidth="28800" windowHeight="11388" activeTab="6" xr2:uid="{550F2F40-7B1A-46CC-9BB7-B3D78208C6B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Neetcode" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Graph" sheetId="7" r:id="rId4"/>
     <sheet name="Sliding window" sheetId="8" r:id="rId5"/>
     <sheet name="AWS" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="92">
   <si>
     <t>Problem</t>
   </si>
@@ -361,6 +362,30 @@
   </si>
   <si>
     <t>Airflow /Orchestration</t>
+  </si>
+  <si>
+    <t>Airflow</t>
+  </si>
+  <si>
+    <t>Pandas / Geopandas</t>
+  </si>
+  <si>
+    <t>Jupyter notebooks</t>
+  </si>
+  <si>
+    <t>Geospatial processing</t>
+  </si>
+  <si>
+    <t>Lidar data</t>
+  </si>
+  <si>
+    <t>Satellite imagery</t>
+  </si>
+  <si>
+    <t>Experience with ArcGIS/QGIS</t>
+  </si>
+  <si>
+    <t>sequence diagrams, class hierarchies, logical system views, etc.</t>
   </si>
 </sst>
 </file>
@@ -480,7 +505,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -531,6 +556,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -548,10 +576,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1046,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95902476-BAA6-400E-B1C6-36D74108E38D}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,7 +1236,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="33" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -1341,7 +1365,7 @@
       </c>
       <c r="I23"/>
     </row>
-    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -1378,6 +1402,62 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56E6154-F7B5-4CA2-AFA7-D11E42E4EC02}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="33" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>